<commit_message>
clarify use of the max uniform parameter
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6403AC-D746-4E0E-980D-1150FD87E2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B894D-BE6C-448B-A5F0-A4BE576791D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="4065" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Description" sheetId="1" r:id="rId1"/>
+    <sheet name="TraitsFile" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -862,18 +862,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA004AD-4C80-44DF-9F9F-43F6D20FCDCD}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -895,7 +895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -917,7 +917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -928,7 +928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -939,7 +939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -950,7 +950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -961,7 +961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -972,7 +972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -983,7 +983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -994,7 +994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1047,26 +1047,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7796729-7AC2-4A22-B345-57AF80AEDFDE}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
doc new OutputValues option
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B894D-BE6C-448B-A5F0-A4BE576791D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCFE189-CCC5-4FA4-A2A4-86925B27208A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>min=0.3,max=1.0</t>
+  </si>
+  <si>
+    <t>OutputValues</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should allele values for this gene be written to output? Ignored if OutputGeneValues in GeneticsFile is set to FALSE. </t>
   </si>
 </sst>
 </file>
@@ -860,20 +869,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA004AD-4C80-44DF-9F9F-43F6D20FCDCD}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -884,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -895,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -906,7 +915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -917,7 +926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -928,7 +937,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -939,7 +948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -950,7 +959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -961,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -972,7 +981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -983,7 +992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1027,7 +1036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1036,6 +1045,17 @@
       </c>
       <c r="C15" s="5" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1051,22 +1071,22 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,7 +1174,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1198,7 +1218,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1242,7 +1262,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1286,7 +1306,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
clarify doc field for OuputValue
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCFE189-CCC5-4FA4-A2A4-86925B27208A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBB0629-2667-4C9B-B8C8-2E9B4E945617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
@@ -435,7 +435,7 @@
     <t>TRUE/FALSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Should allele values for this gene be written to output? Ignored if OutputGeneValues in GeneticsFile is set to FALSE. </t>
+    <t xml:space="preserve">If OutputGeneValues in GeneticsFile is enabled, should allele values for this gene be written to output? Ignored if OutputGeneValues is set to FALSE. </t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
initialise genetic load with non-zero sel + dom coeffs #75
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE388C4-532B-4A61-AC5B-8D0BE3B146E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E984D455-C70E-4357-B885-E602620FA461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>ExpressionType</t>
-  </si>
-  <si>
-    <t>InitialDistribution</t>
-  </si>
-  <si>
-    <t>InitialParameters</t>
   </si>
   <si>
     <t>DominanceDistribution</t>
@@ -251,17 +245,200 @@
     <t>Loci positions coding for trait within genome. Must be in the range 0-(GenomeSize-1), specified in Genetics file. Positions can overlap across traits - there will be no pleiotropy, but this will influence genetic linkage.</t>
   </si>
   <si>
+    <t>Distribution from which to draw the dominance value for mutations from</t>
+  </si>
+  <si>
+    <t>‘uniform’ : min=single float value,max=single float value
+‘normal : mean=single float value,sd=single float value
+‘gamma’ : shape=single float value, scale=single float value
+‘negExp’ : mean=single float value
+‘scaled’ : mean= mean dominance coefficient, single float</t>
+  </si>
+  <si>
+    <t>Dispersal traits only: option to have inter-individual variability in without inheritance, i.e. values at trait loci are re-sampled from initial distribution parameters every generation, not inherited and mutation parameters do not apply.</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE for dispersal, always FALSE for others</t>
+  </si>
+  <si>
+    <t>Distribution for mutations to draw from</t>
+  </si>
+  <si>
+    <t>‘KAM’ : max=single integer value (cannot exceed 255)
+‘SSM’ : max=single integer value (cannot exceed 255)
+‘uniform’ : min=single float value,max=single float value
+‘normal : mean=single float value,sd=single float value
+‘gamma’ : shape=single float value, scale=single float value
+‘negExp’ : mean=single float value</t>
+  </si>
+  <si>
+    <t>Mutation rate applicable to this type of loci</t>
+  </si>
+  <si>
+    <t>Single float value.</t>
+  </si>
+  <si>
+    <t>Neutral : 'KAM' or 'SSM'
+Neutral are coded as chars. KAM (k-alleles model) is randomly draw a value between 0 and max (see MutationParameters). 
+SSM (single-step mutation) is to move in a stepwise manner, A to B, B to C.
+Genetic load:  ‘gamma’, ‘uniform’, ‘normal’,‘negExp’
+Dispersal: ‘uniform’ or‘normal’
+Dispersal trait mutations are cumulative; non-dispersal mutations replace the previous allele value</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>uniform</t>
+  </si>
+  <si>
+    <t>max=2</t>
+  </si>
+  <si>
+    <t>KAM</t>
+  </si>
+  <si>
+    <t>multiplicative</t>
+  </si>
+  <si>
+    <t>scaled</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>emigration_d0</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>min=0.0,max=1.0</t>
+  </si>
+  <si>
+    <t>mean=0,sd=0.2</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>genetic_load</t>
+  </si>
+  <si>
+    <t>mean=0.1</t>
+  </si>
+  <si>
+    <t>shape=0.2,scale=0.15</t>
+  </si>
+  <si>
+    <t>mean=0.5,sd=0.1</t>
+  </si>
+  <si>
+    <t>mean=0.5,sd=0.2</t>
+  </si>
+  <si>
+    <t>min=0.3,max=1.0</t>
+  </si>
+  <si>
+    <t>OutputValues</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If OutputGeneValues in GeneticsFile is enabled, should allele values for this gene be written to output? Ignored if OutputGeneValues is set to FALSE. </t>
+  </si>
+  <si>
+    <t>0-229</t>
+  </si>
+  <si>
+    <t>230-259</t>
+  </si>
+  <si>
+    <t>280-289</t>
+  </si>
+  <si>
+    <t>290-299</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameters for above distributions. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No space around the = sign, or between parameters and commas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameters for the above distribution. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No space around the = sign, or between parameters and commas.</t>
+    </r>
+  </si>
+  <si>
+    <t>InitialAlleleDist</t>
+  </si>
+  <si>
+    <t>InitialAlleleParams</t>
+  </si>
+  <si>
+    <t>InitialDomDist</t>
+  </si>
+  <si>
+    <t>InitialDomParams</t>
+  </si>
+  <si>
+    <t>Neutral: ‘uniform’. Initialise with random characters between 0 – max. Note that possible values start at 0, so 'max=0' specifies a monomorphic initial population.
+Dispersal: ‘uniform’ or ‘normal’ .
+Genetic fitness:  ‘gamma’, ‘uniform’, ‘normal’,‘negExp’, or blank (#), in which case genetic load starts at 0.</t>
+  </si>
+  <si>
     <t>Neutral: ‘uniform’ : max=single integer value
 Dispersal traits:
 ‘uniform’ : min=single float value,max=single float value
-‘normal : mean=single float value,sd=single float value</t>
-  </si>
-  <si>
-    <t>Distribution from which to draw the dominance value for mutations from</t>
-  </si>
-  <si>
-    <r>
-      <t>Not applicable to dispersal or neutral traits.
+‘normal : mean=single float value,sd=single float value
+Genetic fitness:
+‘uniform’ : min=single float value,max=single float value
+‘normal : mean=single float value,sd=single float value
+‘gamma’ : shape=single float value, scale=single float value
+‘negExp’ : mean=single float value
+If InitialAlleleDist is blank, then this must be blank as well.</t>
+  </si>
+  <si>
+    <t>Distribution from which to draw initial dominance coefficients from</t>
+  </si>
+  <si>
+    <r>
+      <t>Not applicable to dispersal or neutral traits, must be blank (#).
 Genetic load: ‘gamma’, ‘uniform’, ‘normal’, ‘negExp’, ‘scaled’ (</t>
     </r>
     <r>
@@ -308,166 +485,22 @@
     </r>
   </si>
   <si>
+    <t>Dispersal or Neutral traits: not applicable, must be blank (#).
+Genetic load: ‘gamma’, ‘uniform’, ‘normal’, ‘negExp’, ‘scaled’ (h depends on s, see cf user manual). Can also be left blank (#), in which case all dominance coefficients start at zero.</t>
+  </si>
+  <si>
     <t>‘uniform’ : min=single float value,max=single float value
 ‘normal : mean=single float value,sd=single float value
 ‘gamma’ : shape=single float value, scale=single float value
 ‘negExp’ : mean=single float value
-‘scaled’ : mean= mean dominance coefficient, single float</t>
-  </si>
-  <si>
-    <t>Dispersal traits only: option to have inter-individual variability in without inheritance, i.e. values at trait loci are re-sampled from initial distribution parameters every generation, not inherited and mutation parameters do not apply.</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE for dispersal, always FALSE for others</t>
-  </si>
-  <si>
-    <t>Distribution for mutations to draw from</t>
-  </si>
-  <si>
-    <t>‘KAM’ : max=single integer value (cannot exceed 255)
-‘SSM’ : max=single integer value (cannot exceed 255)
-‘uniform’ : min=single float value,max=single float value
-‘normal : mean=single float value,sd=single float value
-‘gamma’ : shape=single float value, scale=single float value
-‘negExp’ : mean=single float value</t>
-  </si>
-  <si>
-    <t>Mutation rate applicable to this type of loci</t>
-  </si>
-  <si>
-    <t>Single float value.</t>
-  </si>
-  <si>
-    <t>Neutral : 'KAM' or 'SSM'
-Neutral are coded as chars. KAM (k-alleles model) is randomly draw a value between 0 and max (see MutationParameters). 
-SSM (single-step mutation) is to move in a stepwise manner, A to B, B to C.
-Genetic load:  ‘gamma’, ‘uniform’, ‘normal’,‘negExp’
-Dispersal: ‘uniform’ or‘normal’
-Dispersal trait mutations are cumulative; non-dispersal mutations replace the previous allele value</t>
-  </si>
-  <si>
-    <t>neutral</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>uniform</t>
-  </si>
-  <si>
-    <t>max=2</t>
-  </si>
-  <si>
-    <t>KAM</t>
-  </si>
-  <si>
-    <t>multiplicative</t>
-  </si>
-  <si>
-    <t>scaled</t>
-  </si>
-  <si>
-    <t>gamma</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>emigration_d0</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>average</t>
-  </si>
-  <si>
-    <t>min=0.0,max=1.0</t>
-  </si>
-  <si>
-    <t>mean=0,sd=0.2</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>genetic_load</t>
-  </si>
-  <si>
-    <t>mean=0.1</t>
-  </si>
-  <si>
-    <t>shape=0.2,scale=0.15</t>
-  </si>
-  <si>
-    <t>mean=0.5,sd=0.1</t>
-  </si>
-  <si>
-    <t>mean=0.5,sd=0.2</t>
-  </si>
-  <si>
-    <t>min=0.3,max=1.0</t>
-  </si>
-  <si>
-    <t>OutputValues</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If OutputGeneValues in GeneticsFile is enabled, should allele values for this gene be written to output? Ignored if OutputGeneValues is set to FALSE. </t>
-  </si>
-  <si>
-    <t>0-229</t>
-  </si>
-  <si>
-    <t>230-259</t>
-  </si>
-  <si>
-    <t>280-289</t>
-  </si>
-  <si>
-    <t>290-299</t>
-  </si>
-  <si>
-    <t>Neutral: ‘uniform’. Initialise with random characters between 0 – max. Note that possible values start at 0, so 'max=0' specifies a monomorphic initial population.
-Dispersal: ‘uniform’ or ‘normal’ .
-Not applicable for genetic fitness traits, genetic load starts at 0.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Parameters for above distributions. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No space around the = sign, or between parameters and commas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Parameters for the above distribution. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No space around the = sign, or between parameters and commas.</t>
-    </r>
+‘scaled’ : mean= mean dominance coefficient, single float
+If InitialDomParams is blank, this must be blank as well.</t>
+  </si>
+  <si>
+    <t>shape=1.5,scale=0.0001</t>
+  </si>
+  <si>
+    <t>mean=0.2</t>
   </si>
 </sst>
 </file>
@@ -901,20 +934,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA004AD-4C80-44DF-9F9F-43F6D20FCDCD}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A9" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -925,169 +958,191 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>64</v>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1098,28 +1153,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7796729-7AC2-4A22-B345-57AF80AEDFDE}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1139,265 +1196,301 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2">
         <v>1E-4</v>
       </c>
-      <c r="O2" t="b">
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3">
+        <v>55</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3">
         <v>1E-4</v>
       </c>
-      <c r="O3" t="b">
+      <c r="Q3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4">
+        <v>57</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4">
         <v>1E-4</v>
       </c>
-      <c r="O4" t="b">
+      <c r="Q4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5">
+        <v>51</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5">
         <v>1E-4</v>
       </c>
-      <c r="O5" t="b">
+      <c r="Q5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6">
+        <v>51</v>
+      </c>
+      <c r="N6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6">
         <v>1E-4</v>
       </c>
-      <c r="O6" t="b">
+      <c r="Q6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doc for initial positions
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30306FB0-881E-4299-9DE3-67F2C0316282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C743C0-F958-4FCB-A7B2-F61C86929841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2400" windowWidth="21600" windowHeight="11325" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="90" yWindow="810" windowWidth="21600" windowHeight="11325" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -501,6 +501,31 @@
 ‘negExp’ : mean=single float value
 ‘scaled’ : mean= mean dominance coefficient, single float
 If InitialDomParams is blank, this must be blank as well.</t>
+  </si>
+  <si>
+    <t>InitialPositions</t>
+  </si>
+  <si>
+    <t>NbrInitialPositions</t>
+  </si>
+  <si>
+    <t>0-20</t>
+  </si>
+  <si>
+    <t>240-244</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>For genetic load and neutral traits :  which positions should be initialised. If enabled, the remaining initial value parameters will only be applied to the selected positions, and all other positions will be set to 0. For dispersal traits, all positions must be initialised.</t>
+  </si>
+  <si>
+    <t>Number of initial positions to randomly sample from across the genome</t>
+  </si>
+  <si>
+    <t>For dispersal: 'all'
+For neutral and genetic load: either 'all', '#' (none), 'random', or a semicolon-separated list of integer ranges. For this last option, the positions must be a subset of the values specified for Positions, and is not available if Positions is set to 'random'.</t>
   </si>
 </sst>
 </file>
@@ -588,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -599,6 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -934,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA004AD-4C80-44DF-9F9F-43F6D20FCDCD}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,122 +1052,144 @@
     </row>
     <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1153,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7796729-7AC2-4A22-B345-57AF80AEDFDE}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,18 +1213,20 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1196,40 +1246,46 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1249,40 +1305,46 @@
         <v>35</v>
       </c>
       <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="b">
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2">
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2">
         <v>1E-4</v>
       </c>
-      <c r="Q2" t="b">
+      <c r="S2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1302,7 +1364,7 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -1313,29 +1375,35 @@
       <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="b">
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" t="b">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>69</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>49</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>1E-4</v>
       </c>
-      <c r="Q3" t="b">
+      <c r="S3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1355,40 +1423,46 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>65</v>
       </c>
-      <c r="K4" t="b">
+      <c r="M4" t="b">
         <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" t="s">
-        <v>70</v>
       </c>
       <c r="N4" t="s">
         <v>43</v>
       </c>
       <c r="O4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
         <v>72</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>1E-4</v>
       </c>
-      <c r="Q4" t="b">
+      <c r="S4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1408,40 +1482,46 @@
         <v>46</v>
       </c>
       <c r="G5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>67</v>
       </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="b">
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>43</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>71</v>
       </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5">
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5">
         <v>1E-4</v>
       </c>
-      <c r="Q5" t="b">
+      <c r="S5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1461,38 +1541,116 @@
         <v>46</v>
       </c>
       <c r="G6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>68</v>
       </c>
-      <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="b">
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" t="b">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>71</v>
       </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6">
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6">
         <v>1E-4</v>
       </c>
-      <c r="Q6" t="b">
+      <c r="S6" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
better description for gene expression
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C743C0-F958-4FCB-A7B2-F61C86929841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9492F88-7083-4A73-8BB4-603EAC9CA00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="810" windowWidth="21600" windowHeight="11325" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="10830" yWindow="3675" windowWidth="21600" windowHeight="11235" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -228,11 +228,6 @@
     <t>Expression of loci</t>
   </si>
   <si>
-    <t>For neutral: not expressed, must be left blank ‘#’
-For dispersal: ‘additive’ or ‘average’
-For genetic fitness: ‘multiplicative’</t>
-  </si>
-  <si>
     <t>Distribution from which to draw initial allele values from</t>
   </si>
   <si>
@@ -526,6 +521,11 @@
   <si>
     <t>For dispersal: 'all'
 For neutral and genetic load: either 'all', '#' (none), 'random', or a semicolon-separated list of integer ranges. For this last option, the positions must be a subset of the values specified for Positions, and is not available if Positions is set to 'random'.</t>
+  </si>
+  <si>
+    <t>For neutral: not expressed, must be left blank ‘#’
+For dispersal: ‘additive’ (all allele values are summed) or ‘average’ (allele values are averaged over all positions and allele pairs, if diploid)
+For genetic fitness: ‘multiplicative’: Fitness is determined by the product of all positions. The fitness value of a single position is one minus the value of each allele multiplied by the relative dominance of the allele over its homolog (see user manual for the formula).</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -624,7 +624,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -963,7 +962,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,10 +1021,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1033,13 +1032,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1047,73 +1046,73 @@
         <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1121,10 +1120,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="150" x14ac:dyDescent="0.25">
@@ -1132,10 +1131,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -1143,10 +1142,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1154,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -1165,10 +1164,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,21 +1175,21 @@
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1201,7 +1200,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7796729-7AC2-4A22-B345-57AF80AEDFDE}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -1246,22 +1245,22 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
       <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
-      </c>
-      <c r="L1" t="s">
-        <v>60</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1282,7 +1281,7 @@
         <v>14</v>
       </c>
       <c r="S1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1290,52 +1289,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R2">
         <v>1E-4</v>
@@ -1349,52 +1348,52 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R3">
         <v>1E-4</v>
@@ -1408,52 +1407,52 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
-      </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R4">
         <v>1E-4</v>
@@ -1467,52 +1466,52 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5">
         <v>1E-4</v>
@@ -1526,52 +1525,52 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R6">
         <v>1E-4</v>
@@ -1579,78 +1578,6 @@
       <c r="S6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
round of fixes post merge conflict
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TraitsFile.xlsx
+++ b/doc/Manual/Batchmode/TraitsFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21308F4D-12E4-4C9B-ADF0-FDB7AD8B1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9A58B3-EEC6-4A17-9FBA-DBAFA172F803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{976B70FE-2B97-4614-B764-D7AAC611EF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -624,6 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -961,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA004AD-4C80-44DF-9F9F-43F6D20FCDCD}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A16" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7796729-7AC2-4A22-B345-57AF80AEDFDE}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1225,62 +1226,62 @@
     <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>